<commit_message>
Resolve tiebreak using single
</commit_message>
<xml_diff>
--- a/data/2020-02-18/Senior Cubers Worldwide - Weekly Competition - 2020-02-18.xlsx
+++ b/data/2020-02-18/Senior Cubers Worldwide - Weekly Competition - 2020-02-18.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\WCA\scw-comp\data\2020-02-18\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B9847F7-94E4-4A71-94C9-9A80A5EAAB9A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5886BEF1-285C-4DDA-9B0A-F3C4114AF796}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="3x3x3" sheetId="1" r:id="rId1"/>
@@ -953,11 +953,11 @@
     <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -10587,8 +10587,8 @@
   </sheetPr>
   <dimension ref="A1:L1034"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -10913,7 +10913,7 @@
     </row>
     <row r="11" spans="1:12" ht="12.75">
       <c r="A11" s="23">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B11" s="16" t="s">
         <v>96</v>
@@ -17482,7 +17482,7 @@
   </sheetPr>
   <dimension ref="A1:L1030"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H16" sqref="H16:J17"/>
     </sheetView>
   </sheetViews>
@@ -17717,7 +17717,7 @@
       <c r="C8" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="68" t="s">
+      <c r="D8" s="66" t="s">
         <v>195</v>
       </c>
       <c r="F8" s="19" t="s">
@@ -24307,12 +24307,12 @@
       <c r="A1" s="40" t="s">
         <v>170</v>
       </c>
-      <c r="B1" s="66" t="s">
+      <c r="B1" s="67" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
       <c r="F1" s="6" t="s">
         <v>171</v>
       </c>

</xml_diff>

<commit_message>
Fix minor data issues
</commit_message>
<xml_diff>
--- a/data/2020-02-18/Senior Cubers Worldwide - Weekly Competition - 2020-02-18.xlsx
+++ b/data/2020-02-18/Senior Cubers Worldwide - Weekly Competition - 2020-02-18.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\WCA\scw-comp\data\2020-02-18\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{622720A2-A69B-436B-8717-FBDC8042F278}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{914A8A0E-C476-49EB-9D70-BC6D001440D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="3x3x3" sheetId="1" r:id="rId1"/>
-    <sheet name="3x3x3 OH" sheetId="2" r:id="rId2"/>
+    <sheet name="OH" sheetId="2" r:id="rId2"/>
     <sheet name="5x5x5" sheetId="3" r:id="rId3"/>
     <sheet name="FMC" sheetId="4" r:id="rId4"/>
   </sheets>
@@ -10589,7 +10589,7 @@
   <dimension ref="A1:L1034"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>

</xml_diff>